<commit_message>
update pension data of Mar_2023
</commit_message>
<xml_diff>
--- a/jupyter/경쟁사.xlsx
+++ b/jupyter/경쟁사.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hr\jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7E74FD-53CA-4F75-87C0-95BE2B418CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70C2789-6602-4E19-B92A-7305A14E0BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{093692AB-55B6-43FA-93B5-1F6AA8C8F403}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{093692AB-55B6-43FA-93B5-1F6AA8C8F403}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>현대자동차(주)</t>
   </si>
@@ -137,6 +137,15 @@
   <si>
     <t>사업장명</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에이치디현대사이트솔루션 주식회사</t>
+  </si>
+  <si>
+    <t>에이치디현대인프라코어(주)</t>
+  </si>
+  <si>
+    <t>에이치디현대건설기계(주)</t>
   </si>
 </sst>
 </file>
@@ -512,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC78CE46-D362-4062-B760-BAD4FBB186CF}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -710,6 +719,39 @@
         <v>30</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1">
+        <v>493810</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1">
+        <v>121814</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1">
+        <v>528880</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>